<commit_message>
Fix to use us labels attribute for filtering scif and use product_pk  for filtering in scene_matches
</commit_message>
<xml_diff>
--- a/Projects/KCUS/Data/KEngine_KC_US_V6.xlsx
+++ b/Projects/KCUS/Data/KEngine_KC_US_V6.xlsx
@@ -22,6 +22,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Original Customer questions'!$F$1:$F$46</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Original Customer questions'!$F$1:$F$46</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Original Customer questions'!$F$1:$F$46</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Original Customer questions'!$F$1:$F$46</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -420,10 +421,10 @@
     <t xml:space="preserve">Category Space - Feminine Needs</t>
   </si>
   <si>
+    <t xml:space="preserve">Feminine Needs</t>
+  </si>
+  <si>
     <t xml:space="preserve">FEM CARE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feminine Needs</t>
   </si>
   <si>
     <t xml:space="preserve">Category Space - Feminine Hygiene</t>
@@ -2766,29 +2767,27 @@
   <dimension ref="1:32"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="I8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.57085020242915"/>
@@ -3983,7 +3982,7 @@
         <v>127</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>125</v>
@@ -3992,13 +3991,13 @@
         <v>32</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>119</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4009,7 +4008,7 @@
         <v>130</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>125</v>
@@ -4018,7 +4017,7 @@
         <v>32</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>119</v>
@@ -4051,18 +4050,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.8421052631579"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="64.2712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9386,22 +9385,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0242914979757"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="40.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="40.7044534412955"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9918,11 +9917,11 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.3724696356275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.0161943319838"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -10710,10 +10709,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="79.1619433198381"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="30" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -10811,7 +10810,7 @@
         <v>491</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D8" s="40"/>
     </row>
@@ -10823,7 +10822,7 @@
         <v>491</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>493</v>
@@ -10837,7 +10836,7 @@
         <v>491</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>495</v>

</xml_diff>